<commit_message>
Final sap flow upscaling analysis
</commit_message>
<xml_diff>
--- a/Data/Pfyn/Pfyn_DBH_2023.xlsx
+++ b/Data/Pfyn/Pfyn_DBH_2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis/Documents/WSL/Project/DeepDrought/Data/Pfyn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60997D14-0C3F-3241-AEFA-D274A20A082A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB8809E-15A4-2146-B572-BA0D5D93139E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{9898B4AF-4A5A-694D-AE34-7557CFA6D8BF}"/>
   </bookViews>
@@ -446,7 +446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B1E344-9B4D-1445-9AEF-05696F71AFA4}">
   <dimension ref="A1:E869"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E459" sqref="E459:E463"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1759,7 +1761,7 @@
         <v>9</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -1776,7 +1778,7 @@
         <v>9</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -1793,7 +1795,7 @@
         <v>9</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -1827,7 +1829,7 @@
         <v>9</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -2456,7 +2458,7 @@
         <v>9</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -2473,7 +2475,7 @@
         <v>9</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
@@ -2490,7 +2492,7 @@
         <v>9</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -2507,7 +2509,7 @@
         <v>9</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -2524,7 +2526,7 @@
         <v>9</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -2541,7 +2543,7 @@
         <v>9</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -2558,7 +2560,7 @@
         <v>9</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -2575,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -2592,7 +2594,7 @@
         <v>9</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -2609,7 +2611,7 @@
         <v>9</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -2626,7 +2628,7 @@
         <v>9</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -2643,7 +2645,7 @@
         <v>9</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -2660,7 +2662,7 @@
         <v>9</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -2677,7 +2679,7 @@
         <v>9</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -2694,7 +2696,7 @@
         <v>9</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -2711,7 +2713,7 @@
         <v>9</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -2728,7 +2730,7 @@
         <v>9</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -2745,7 +2747,7 @@
         <v>9</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -2762,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -2779,7 +2781,7 @@
         <v>9</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -2796,7 +2798,7 @@
         <v>9</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -2813,7 +2815,7 @@
         <v>9</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -2830,7 +2832,7 @@
         <v>9</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -2847,7 +2849,7 @@
         <v>9</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -2864,7 +2866,7 @@
         <v>9</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -2881,7 +2883,7 @@
         <v>9</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -2898,7 +2900,7 @@
         <v>9</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -2915,7 +2917,7 @@
         <v>9</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -2932,7 +2934,7 @@
         <v>9</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -2949,7 +2951,7 @@
         <v>9</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -2966,7 +2968,7 @@
         <v>9</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -2983,7 +2985,7 @@
         <v>9</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -3000,7 +3002,7 @@
         <v>9</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -3017,7 +3019,7 @@
         <v>9</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -3034,7 +3036,7 @@
         <v>9</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -3051,7 +3053,7 @@
         <v>9</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -6026,7 +6028,7 @@
         <v>9</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
@@ -6043,7 +6045,7 @@
         <v>9</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
@@ -6060,7 +6062,7 @@
         <v>9</v>
       </c>
       <c r="E330" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
@@ -6077,7 +6079,7 @@
         <v>9</v>
       </c>
       <c r="E331" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
@@ -6094,7 +6096,7 @@
         <v>9</v>
       </c>
       <c r="E332" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
@@ -6111,7 +6113,7 @@
         <v>9</v>
       </c>
       <c r="E333" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
@@ -6128,7 +6130,7 @@
         <v>9</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
@@ -6145,7 +6147,7 @@
         <v>9</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
@@ -6162,7 +6164,7 @@
         <v>9</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
@@ -6179,7 +6181,7 @@
         <v>9</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
@@ -6196,7 +6198,7 @@
         <v>9</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
@@ -6213,7 +6215,7 @@
         <v>9</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.2">
@@ -6230,7 +6232,7 @@
         <v>9</v>
       </c>
       <c r="E340" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
@@ -6247,7 +6249,7 @@
         <v>9</v>
       </c>
       <c r="E341" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
@@ -6264,7 +6266,7 @@
         <v>9</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
@@ -6281,7 +6283,7 @@
         <v>9</v>
       </c>
       <c r="E343" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.2">
@@ -6298,7 +6300,7 @@
         <v>9</v>
       </c>
       <c r="E344" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
@@ -6315,7 +6317,7 @@
         <v>9</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
@@ -6332,7 +6334,7 @@
         <v>9</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.2">
@@ -6349,7 +6351,7 @@
         <v>9</v>
       </c>
       <c r="E347" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
@@ -6502,7 +6504,7 @@
         <v>9</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.2">
@@ -7029,7 +7031,7 @@
         <v>9</v>
       </c>
       <c r="E387" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
@@ -7046,7 +7048,7 @@
         <v>9</v>
       </c>
       <c r="E388" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
@@ -7063,7 +7065,7 @@
         <v>9</v>
       </c>
       <c r="E389" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.2">
@@ -7080,7 +7082,7 @@
         <v>9</v>
       </c>
       <c r="E390" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
@@ -7097,7 +7099,7 @@
         <v>9</v>
       </c>
       <c r="E391" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.2">
@@ -7131,7 +7133,7 @@
         <v>9</v>
       </c>
       <c r="E393" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.2">
@@ -7148,7 +7150,7 @@
         <v>9</v>
       </c>
       <c r="E394" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.2">
@@ -7165,7 +7167,7 @@
         <v>9</v>
       </c>
       <c r="E395" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
@@ -7182,7 +7184,7 @@
         <v>9</v>
       </c>
       <c r="E396" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
@@ -7199,7 +7201,7 @@
         <v>9</v>
       </c>
       <c r="E397" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.2">
@@ -7216,7 +7218,7 @@
         <v>9</v>
       </c>
       <c r="E398" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.2">
@@ -7233,7 +7235,7 @@
         <v>9</v>
       </c>
       <c r="E399" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.2">
@@ -7250,7 +7252,7 @@
         <v>9</v>
       </c>
       <c r="E400" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.2">
@@ -7267,7 +7269,7 @@
         <v>9</v>
       </c>
       <c r="E401" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.2">
@@ -7284,7 +7286,7 @@
         <v>9</v>
       </c>
       <c r="E402" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.2">
@@ -7301,7 +7303,7 @@
         <v>9</v>
       </c>
       <c r="E403" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.2">
@@ -7318,7 +7320,7 @@
         <v>9</v>
       </c>
       <c r="E404" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.2">
@@ -7641,7 +7643,7 @@
         <v>9</v>
       </c>
       <c r="E423" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.2">
@@ -7658,7 +7660,7 @@
         <v>9</v>
       </c>
       <c r="E424" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.2">
@@ -7675,7 +7677,7 @@
         <v>9</v>
       </c>
       <c r="E425" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.2">
@@ -7692,7 +7694,7 @@
         <v>9</v>
       </c>
       <c r="E426" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.2">
@@ -7709,7 +7711,7 @@
         <v>9</v>
       </c>
       <c r="E427" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.2">
@@ -7726,7 +7728,7 @@
         <v>9</v>
       </c>
       <c r="E428" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.2">
@@ -7743,7 +7745,7 @@
         <v>9</v>
       </c>
       <c r="E429" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.2">
@@ -7760,7 +7762,7 @@
         <v>9</v>
       </c>
       <c r="E430" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.2">
@@ -7777,7 +7779,7 @@
         <v>9</v>
       </c>
       <c r="E431" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.2">
@@ -7794,7 +7796,7 @@
         <v>9</v>
       </c>
       <c r="E432" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.2">
@@ -7811,7 +7813,7 @@
         <v>9</v>
       </c>
       <c r="E433" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.2">
@@ -7828,7 +7830,7 @@
         <v>9</v>
       </c>
       <c r="E434" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.2">
@@ -7845,7 +7847,7 @@
         <v>9</v>
       </c>
       <c r="E435" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.2">
@@ -7862,7 +7864,7 @@
         <v>9</v>
       </c>
       <c r="E436" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.2">
@@ -8253,7 +8255,7 @@
         <v>9</v>
       </c>
       <c r="E459" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.2">
@@ -8270,7 +8272,7 @@
         <v>9</v>
       </c>
       <c r="E460" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.2">
@@ -8287,7 +8289,7 @@
         <v>9</v>
       </c>
       <c r="E461" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.2">
@@ -8304,7 +8306,7 @@
         <v>9</v>
       </c>
       <c r="E462" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.2">
@@ -8321,7 +8323,7 @@
         <v>9</v>
       </c>
       <c r="E463" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>